<commit_message>
change file name to english, add summary of collection & iterator
</commit_message>
<xml_diff>
--- a/all.xlsx
+++ b/all.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>技术</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,6 +46,38 @@
   </si>
   <si>
     <t>doc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运算符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deque</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迭代器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChainMap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -53,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +95,28 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -89,8 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -371,14 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -406,8 +466,92 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>50</v>
+      <c r="D2" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>